<commit_message>
Changes at the end of 10-8 AM
</commit_message>
<xml_diff>
--- a/Plex_Bot/Movement planner.xlsx
+++ b/Plex_Bot/Movement planner.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -237,13 +237,13 @@
   </sheetPr>
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X5" activeCellId="0" sqref="X5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U17" activeCellId="0" sqref="B2:U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.89795918367347"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.69897959183673"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
@@ -411,7 +411,7 @@
         <v>11</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>11</v>
@@ -451,64 +451,64 @@
       <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="P4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="R4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="T4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" s="0" t="s">
+      <c r="B4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>-10</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>-10</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>-20</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="X4" s="0" t="s">
@@ -523,13 +523,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>11</v>
@@ -547,13 +547,13 @@
         <v>11</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>11</v>
@@ -565,19 +565,19 @@
         <v>11</v>
       </c>
       <c r="P5" s="1" t="n">
-        <v>0</v>
+        <v>-40</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="R5" s="1" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="T5" s="1" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>11</v>
@@ -587,64 +587,64 @@
       <c r="A6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="P6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="R6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="T6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" s="0" t="s">
+      <c r="B6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>-20</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>-15</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>-40</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -653,61 +653,61 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J7" s="1" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="N7" s="1" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P7" s="1" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="R7" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="T7" s="1" t="n">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>11</v>
@@ -717,62 +717,62 @@
       <c r="A8" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="N8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="P8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="R8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="T8" s="0" t="n">
-        <v>0</v>
+      <c r="B8" s="1" t="n">
+        <v>-15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P8" s="1" t="n">
+        <v>-20</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T8" s="1" t="n">
+        <v>-10</v>
       </c>
       <c r="U8" s="0" t="s">
         <v>11</v>

</xml_diff>